<commit_message>
polishing plots and result output
</commit_message>
<xml_diff>
--- a/examples/ww_tibnine_dewatered_sludge_input_preparation.xlsx
+++ b/examples/ww_tibnine_dewatered_sludge_input_preparation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\OneDrive\Desktop\Doctorate\Case Studies\Renewable Energy from Wastewater_Lebanon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\OWEFE\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{67608FBC-3A67-4920-97E1-A4558AB6161F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4009AB3-94A1-41B3-8D8C-B0B43839459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Wastewate Flow [m³/month] (2020)</t>
   </si>
@@ -91,12 +91,15 @@
   </si>
   <si>
     <t>ds [m³/day) without conversion factor and exact day adoption</t>
+  </si>
+  <si>
+    <t>Total Sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,11 +447,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,7 +494,7 @@
         <v>30.913978494623656</v>
       </c>
       <c r="E2" s="1">
-        <f>C2/(1.02*0.997)</f>
+        <f t="shared" ref="E2:E13" si="0">C2/(1.02*0.997)</f>
         <v>22.616870218498633</v>
       </c>
       <c r="F2" s="1"/>
@@ -511,7 +514,7 @@
         <v>47.197640117994098</v>
       </c>
       <c r="E3" s="1">
-        <f>C3/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>31.46694986921549</v>
       </c>
       <c r="F3" s="1"/>
@@ -531,7 +534,7 @@
         <v>57.795698924731184</v>
       </c>
       <c r="E4" s="1">
-        <f>C4/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>42.283713886758314</v>
       </c>
       <c r="F4" s="1"/>
@@ -551,7 +554,7 @@
         <v>68.055555555555557</v>
       </c>
       <c r="E5" s="1">
-        <f>C5/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>48.183766987236218</v>
       </c>
       <c r="F5" s="1"/>
@@ -571,7 +574,7 @@
         <v>67.204301075268816</v>
       </c>
       <c r="E6" s="1">
-        <f>C6/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>49.167109170649205</v>
       </c>
       <c r="F6" s="1"/>
@@ -591,7 +594,7 @@
         <v>77.777777777777771</v>
       </c>
       <c r="E7" s="1">
-        <f>C7/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>55.06716227112711</v>
       </c>
       <c r="F7" s="1"/>
@@ -611,7 +614,7 @@
         <v>99.462365591397855</v>
       </c>
       <c r="E8" s="1">
-        <f>C8/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>72.767321572560817</v>
       </c>
       <c r="F8" s="1"/>
@@ -631,7 +634,7 @@
         <v>111.55913978494624</v>
       </c>
       <c r="E9" s="1">
-        <f>C9/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>81.617401223277682</v>
       </c>
       <c r="F9" s="1"/>
@@ -651,7 +654,7 @@
         <v>111.11111111111111</v>
       </c>
       <c r="E10" s="1">
-        <f>C10/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>78.667374673038722</v>
       </c>
       <c r="F10" s="1"/>
@@ -671,7 +674,7 @@
         <v>60.483870967741936</v>
       </c>
       <c r="E11" s="1">
-        <f>C11/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>44.250398253584287</v>
       </c>
       <c r="F11" s="1"/>
@@ -691,7 +694,7 @@
         <v>48.611111111111114</v>
       </c>
       <c r="E12" s="1">
-        <f>C12/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>34.416976419454443</v>
       </c>
       <c r="F12" s="1"/>
@@ -711,7 +714,7 @@
         <v>76.612903225806448</v>
       </c>
       <c r="E13" s="1">
-        <f>C13/(1.02*0.997)</f>
+        <f t="shared" si="0"/>
         <v>56.050504454540096</v>
       </c>
       <c r="F13" s="1"/>
@@ -733,6 +736,15 @@
         <v>71.398787811505471</v>
       </c>
       <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C2:C13)</f>
+        <v>627</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">

</xml_diff>

<commit_message>
update digester CSTR according to design approach of Jean
</commit_message>
<xml_diff>
--- a/examples/ww_tibnine_dewatered_sludge_input_preparation.xlsx
+++ b/examples/ww_tibnine_dewatered_sludge_input_preparation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\OWEFE\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\PycharmProjects\OWEFE\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4009AB3-94A1-41B3-8D8C-B0B43839459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A327EA9-844F-4DB5-9896-59B48830E284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="1900" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,10 @@
     <t>dewatered sludge (m³/day)</t>
   </si>
   <si>
-    <t>ds [m³/day) without conversion factor and exact day adoption</t>
-  </si>
-  <si>
     <t>Total Sum</t>
+  </si>
+  <si>
+    <t>ds [t/day), without exact day adaption</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -739,15 +739,15 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <f>SUM(C2:C13)</f>
         <v>627</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+    <row r="16" spans="1:6" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="1">
@@ -761,7 +761,7 @@
     </row>
     <row r="17" spans="2:3" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <f>C14/30</f>

</xml_diff>